<commit_message>
created AXI SPI writer
</commit_message>
<xml_diff>
--- a/FPGA/documentation/Codec SPI Write Timing Diag.xlsx
+++ b/FPGA/documentation/Codec SPI Write Timing Diag.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xilinxdesigns\Saturn\FPGA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634F8FA3-6470-4AC2-A629-BFD7A4E884B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD157F25-135A-4CEC-A5B6-B44BA8410A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C7A3D78-50A8-4E33-8D42-435C0A15A8C9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>AXI SPI Writer /timing Diagram</t>
   </si>
@@ -67,9 +67,6 @@
     <t>SPIBusy</t>
   </si>
   <si>
-    <t>SPILoad</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -158,6 +155,12 @@
   </si>
   <si>
     <t>on entry to state 5: assert SPILoad</t>
+  </si>
+  <si>
+    <t>SPILoad0</t>
+  </si>
+  <si>
+    <t>ClearValid</t>
   </si>
 </sst>
 </file>
@@ -189,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -292,11 +295,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -308,6 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -323,6 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,10 +669,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AO35"/>
+  <dimension ref="A1:AO37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="AF28" sqref="AF28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +795,7 @@
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -815,81 +844,81 @@
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13" t="s">
+      <c r="H17" s="13"/>
+      <c r="I17" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13" t="s">
+      <c r="J17" s="13"/>
+      <c r="K17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13" t="s">
+      <c r="L17" s="13"/>
+      <c r="M17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="13" t="s">
+      <c r="N17" s="13"/>
+      <c r="O17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N17" s="12"/>
-      <c r="O17" s="13" t="s">
+      <c r="P17" s="13"/>
+      <c r="Q17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="13" t="s">
+      <c r="R17" s="13"/>
+      <c r="S17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="R17" s="12"/>
-      <c r="S17" s="13" t="s">
+      <c r="T17" s="13"/>
+      <c r="U17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="T17" s="12"/>
-      <c r="U17" s="13" t="s">
+      <c r="V17" s="13"/>
+      <c r="W17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="V17" s="12"/>
-      <c r="W17" s="13" t="s">
+      <c r="X17" s="13"/>
+      <c r="Y17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="13" t="s">
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="13" t="s">
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AB17" s="12"/>
-      <c r="AC17" s="13" t="s">
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AD17" s="12"/>
-      <c r="AE17" s="13" t="s">
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AF17" s="12"/>
-      <c r="AG17" s="13" t="s">
+      <c r="AH17" s="13"/>
+      <c r="AI17" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="AH17" s="12"/>
-      <c r="AI17" s="13" t="s">
+      <c r="AJ17" s="13"/>
+      <c r="AK17" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AJ17" s="12"/>
-      <c r="AK17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL17" s="11"/>
+      <c r="AL17" s="12"/>
       <c r="AM17" s="6"/>
       <c r="AN17" s="6"/>
       <c r="AO17" s="6"/>
@@ -933,20 +962,62 @@
       <c r="AH19" s="4"/>
       <c r="AI19" s="4"/>
       <c r="AJ19" s="4"/>
-      <c r="AK19" s="8"/>
+      <c r="AK19" s="15"/>
       <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
     </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="7"/>
+      <c r="AK20" s="7"/>
+      <c r="AL20" s="7"/>
+      <c r="AM20" s="7"/>
+      <c r="AN20" s="7"/>
+      <c r="AO20" s="7"/>
+    </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -977,256 +1048,305 @@
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-      <c r="AJ21" s="2"/>
+      <c r="AJ21" s="9"/>
       <c r="AK21" s="2"/>
-      <c r="AL21" s="3"/>
-      <c r="AM21" s="4"/>
-      <c r="AN21" s="4"/>
-      <c r="AO21" s="4"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="4"/>
+      <c r="AN23" s="4"/>
+      <c r="AO23" s="4"/>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <v>3</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2</v>
+      </c>
+      <c r="H25" s="5">
+        <v>3</v>
+      </c>
+      <c r="I25" s="5">
+        <v>2</v>
+      </c>
+      <c r="J25" s="5">
+        <v>3</v>
+      </c>
+      <c r="K25" s="5">
+        <v>2</v>
+      </c>
+      <c r="L25" s="5">
+        <v>3</v>
+      </c>
+      <c r="M25" s="5">
+        <v>2</v>
+      </c>
+      <c r="N25" s="5">
+        <v>3</v>
+      </c>
+      <c r="O25" s="5">
+        <v>2</v>
+      </c>
+      <c r="P25" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>2</v>
+      </c>
+      <c r="R25" s="5">
+        <v>3</v>
+      </c>
+      <c r="S25" s="5">
+        <v>2</v>
+      </c>
+      <c r="T25" s="5">
+        <v>3</v>
+      </c>
+      <c r="U25" s="5">
+        <v>2</v>
+      </c>
+      <c r="V25" s="5">
+        <v>3</v>
+      </c>
+      <c r="W25" s="5">
+        <v>2</v>
+      </c>
+      <c r="X25" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y25" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z25" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA25" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB25" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC25" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD25" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE25" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF25" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG25" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH25" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI25" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ25" s="5">
+        <v>3</v>
+      </c>
+      <c r="AK25" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL25" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM25" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="5">
+      <c r="E26" s="10">
+        <v>15</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="10">
+        <v>14</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="10">
+        <v>13</v>
+      </c>
+      <c r="J26" s="11"/>
+      <c r="K26" s="10">
+        <v>12</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="10">
+        <v>11</v>
+      </c>
+      <c r="N26" s="11"/>
+      <c r="O26" s="10">
+        <v>10</v>
+      </c>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="10">
+        <v>9</v>
+      </c>
+      <c r="R26" s="11"/>
+      <c r="S26" s="10">
+        <v>8</v>
+      </c>
+      <c r="T26" s="11"/>
+      <c r="U26" s="10">
+        <v>7</v>
+      </c>
+      <c r="V26" s="11"/>
+      <c r="W26" s="10">
+        <v>6</v>
+      </c>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="10">
+        <v>5</v>
+      </c>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="10">
+        <v>4</v>
+      </c>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="10">
+        <v>3</v>
+      </c>
+      <c r="AD26" s="11"/>
+      <c r="AE26" s="10">
+        <v>2</v>
+      </c>
+      <c r="AF26" s="11"/>
+      <c r="AG26" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="11"/>
+      <c r="AI26" s="10">
         <v>0</v>
       </c>
-      <c r="C23" s="5">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
-        <v>1</v>
-      </c>
-      <c r="F23" s="5">
-        <v>3</v>
-      </c>
-      <c r="G23" s="5">
-        <v>2</v>
-      </c>
-      <c r="H23" s="5">
-        <v>3</v>
-      </c>
-      <c r="I23" s="5">
-        <v>2</v>
-      </c>
-      <c r="J23" s="5">
-        <v>3</v>
-      </c>
-      <c r="K23" s="5">
-        <v>2</v>
-      </c>
-      <c r="L23" s="5">
-        <v>3</v>
-      </c>
-      <c r="M23" s="5">
-        <v>2</v>
-      </c>
-      <c r="N23" s="5">
-        <v>3</v>
-      </c>
-      <c r="O23" s="5">
-        <v>2</v>
-      </c>
-      <c r="P23" s="5">
-        <v>3</v>
-      </c>
-      <c r="Q23" s="5">
-        <v>2</v>
-      </c>
-      <c r="R23" s="5">
-        <v>3</v>
-      </c>
-      <c r="S23" s="5">
-        <v>2</v>
-      </c>
-      <c r="T23" s="5">
-        <v>3</v>
-      </c>
-      <c r="U23" s="5">
-        <v>2</v>
-      </c>
-      <c r="V23" s="5">
-        <v>3</v>
-      </c>
-      <c r="W23" s="5">
-        <v>2</v>
-      </c>
-      <c r="X23" s="5">
-        <v>3</v>
-      </c>
-      <c r="Y23" s="5">
-        <v>2</v>
-      </c>
-      <c r="Z23" s="5">
-        <v>3</v>
-      </c>
-      <c r="AA23" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB23" s="5">
-        <v>3</v>
-      </c>
-      <c r="AC23" s="5">
-        <v>2</v>
-      </c>
-      <c r="AD23" s="5">
-        <v>3</v>
-      </c>
-      <c r="AE23" s="5">
-        <v>2</v>
-      </c>
-      <c r="AF23" s="5">
-        <v>3</v>
-      </c>
-      <c r="AG23" s="5">
-        <v>2</v>
-      </c>
-      <c r="AH23" s="5">
-        <v>3</v>
-      </c>
-      <c r="AI23" s="5">
-        <v>2</v>
-      </c>
-      <c r="AJ23" s="5">
-        <v>3</v>
-      </c>
-      <c r="AK23" s="5">
-        <v>4</v>
-      </c>
-      <c r="AL23" s="5">
-        <v>5</v>
-      </c>
-      <c r="AM23" s="5">
-        <v>0</v>
-      </c>
-      <c r="AN23" s="5">
-        <v>0</v>
-      </c>
-      <c r="AO23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="9">
-        <v>15</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="9">
-        <v>14</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="9">
-        <v>13</v>
-      </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="9">
-        <v>12</v>
-      </c>
-      <c r="L24" s="10"/>
-      <c r="M24" s="9">
-        <v>11</v>
-      </c>
-      <c r="N24" s="10"/>
-      <c r="O24" s="9">
-        <v>10</v>
-      </c>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="9">
-        <v>9</v>
-      </c>
-      <c r="R24" s="10"/>
-      <c r="S24" s="9">
-        <v>8</v>
-      </c>
-      <c r="T24" s="10"/>
-      <c r="U24" s="9">
-        <v>7</v>
-      </c>
-      <c r="V24" s="10"/>
-      <c r="W24" s="9">
-        <v>6</v>
-      </c>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="9">
-        <v>5</v>
-      </c>
-      <c r="Z24" s="10"/>
-      <c r="AA24" s="9">
-        <v>4</v>
-      </c>
-      <c r="AB24" s="10"/>
-      <c r="AC24" s="9">
-        <v>3</v>
-      </c>
-      <c r="AD24" s="10"/>
-      <c r="AE24" s="9">
-        <v>2</v>
-      </c>
-      <c r="AF24" s="10"/>
-      <c r="AG24" s="9">
-        <v>1</v>
-      </c>
-      <c r="AH24" s="10"/>
-      <c r="AI24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="10"/>
-    </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
+      <c r="AJ26" s="11"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>34</v>
+      <c r="A29" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="AE26:AF26"/>
+    <mergeCell ref="AG26:AH26"/>
     <mergeCell ref="AI17:AJ17"/>
     <mergeCell ref="AK17:AL17"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
     <mergeCell ref="Q17:R17"/>
     <mergeCell ref="S17:T17"/>
     <mergeCell ref="U17:V17"/>
@@ -1234,26 +1354,22 @@
     <mergeCell ref="Y17:Z17"/>
     <mergeCell ref="AA17:AB17"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="AI26:AJ26"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Y26:Z26"/>
     <mergeCell ref="AC17:AD17"/>
     <mergeCell ref="AE17:AF17"/>
     <mergeCell ref="AG17:AH17"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="AA24:AB24"/>
-    <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="AE24:AF24"/>
-    <mergeCell ref="AG24:AH24"/>
-    <mergeCell ref="AI24:AJ24"/>
+    <mergeCell ref="AA26:AB26"/>
+    <mergeCell ref="AC26:AD26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>